<commit_message>
🔧 Fixed Stray Dog scraper and updated workflows
</commit_message>
<xml_diff>
--- a/gym_data.xlsx
+++ b/gym_data.xlsx
@@ -567,9 +567,9 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>https://tokofitness.id/wp-content/uploads/2019/05/download-500x671.png</t>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD...</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
@@ -648,12 +648,11 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F2" r:id="rId2"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E3" r:id="rId3"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F3" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E4" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E5" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E6" r:id="rId9"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E5" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E6" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -758,7 +757,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Price not available</t>
+          <t>$459.99</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">

</xml_diff>

<commit_message>
🚀 Updated scrapers & data for latest prices
</commit_message>
<xml_diff>
--- a/gym_data.xlsx
+++ b/gym_data.xlsx
@@ -567,9 +567,9 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD...</t>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>https://garagegymlab.com/wp-content/uploads/Rogue-RM-3-Monster-Rack-2.0-Blue.jpg</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
@@ -648,11 +648,12 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F2" r:id="rId2"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E3" r:id="rId3"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F3" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E5" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E6" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E4" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E5" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E6" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -821,7 +822,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Not Available</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -836,7 +837,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Not Available</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated scrapers 2, 3, and 7; refreshed gym data and report
</commit_message>
<xml_diff>
--- a/gym_data.xlsx
+++ b/gym_data.xlsx
@@ -495,7 +495,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$2,056.00</t>
+          <t>$2,070.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -527,7 +527,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>$1,119.99</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$1,487.00</t>
+          <t>$1,497.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">

</xml_diff>

<commit_message>
🛠 Updated placeholder images and integrated Leg Extensions into main and app
</commit_message>
<xml_diff>
--- a/gym_data.xlsx
+++ b/gym_data.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="4x4 Squat Racks" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Squat Stands" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Leg Extensions" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -495,7 +496,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$2,087.00</t>
+          <t>$2,072.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -527,7 +528,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>$1,119.99</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -726,7 +727,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$1,509.00</t>
+          <t>$1,498.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -758,7 +759,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Price not available</t>
+          <t>$459.99</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -887,4 +888,233 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="35" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Product Name</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Manufacturer</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Image URL</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Product Page</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>No Leg Extension Available</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Oak Club MFG</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Not Available</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>https://t3.ftcdn.net/jpg/01/12/43/90/360_F_112439022_Sft6cXK9GLnzWjjIkVMj2Lt34RcKUpxm.jpg</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Not Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Leg Extension and Curl Machine | 10 - 250 LB Selector</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Titan Fitness</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$2,529.99</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>https://titan.fitness/cdn/shop/files/401926_01.jpg?v=1739302160&amp;width=832</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>https://titan.fitness/products/selectorized-leg-extension-and-curl-machine</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>No Leg Extension Available</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Rogue Fitness</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Not Available</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>https://t3.ftcdn.net/jpg/01/12/43/90/360_F_112439022_Sft6cXK9GLnzWjjIkVMj2Lt34RcKUpxm.jpg</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Not Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Selectorized Seated Leg Curl/Extension</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Stray Dog Strength</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$5,250.00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>https://shop.straydogstrength.com/cdn/shop/files/2325-RIGHT-RED_eee5d4da-9504-4bb9-b7e3-f98e7e85c231.jpg?v=1743705611&amp;width=823</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>https://shop.straydogstrength.com/products/selectorized-seated-leg-curl-extension</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>LEG EXTENSION / CURL MACHINE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Sorinex</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$4,149.00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>https://cdn.shopify.com/s/files/1/2559/4942/files/LegCurlLegExtension.jpg?v=1733930466</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>https://www.sorinex.com/products/leg-extension-curl-machine?Title=Default+Title</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F3" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E4" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E5" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E6" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Initial commit - Gym Scraper App
</commit_message>
<xml_diff>
--- a/gym_data.xlsx
+++ b/gym_data.xlsx
@@ -496,7 +496,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$2,072.00</t>
+          <t>$2,137.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -528,7 +528,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$1,119.99</t>
+          <t>$1,299.99</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -727,7 +727,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$1,498.00</t>
+          <t>$1,545.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -759,7 +759,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$459.99</t>
+          <t>$528.99</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -989,7 +989,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$2,529.99</t>
+          <t>$2,909.99</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">

</xml_diff>